<commit_message>
Table - Bands Sensors Fix
New version of bands sensor
</commit_message>
<xml_diff>
--- a/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
+++ b/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Repos\StopCortaderiaLife\DATA\TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C51FF72F-6D3C-477A-8FE7-AD1CF5299D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0DEBCF-E2A4-488E-9355-BB51FC3FB4C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
   <si>
     <t>Blue</t>
   </si>
@@ -99,10 +100,145 @@
     <t>RedEdgeMx</t>
   </si>
   <si>
-    <t>Res (m)(a 120m)</t>
-  </si>
-  <si>
     <t>Parrot Sequoia</t>
+  </si>
+  <si>
+    <t>RapidEye</t>
+  </si>
+  <si>
+    <t>Ikonos</t>
+  </si>
+  <si>
+    <t>Geoeye 1</t>
+  </si>
+  <si>
+    <t>Planet - Dove 1 to 4</t>
+  </si>
+  <si>
+    <t>SPOT 6 and 7</t>
+  </si>
+  <si>
+    <t>Kompsat 2, 3 and 3A</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Worldview-2 and 3</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Spatial_res</t>
+  </si>
+  <si>
+    <t>Blue_min</t>
+  </si>
+  <si>
+    <t>Blue_max</t>
+  </si>
+  <si>
+    <t>Green_min</t>
+  </si>
+  <si>
+    <t>Green_max</t>
+  </si>
+  <si>
+    <t>Red_min</t>
+  </si>
+  <si>
+    <t>Red_max</t>
+  </si>
+  <si>
+    <t>Sentinel-2</t>
+  </si>
+  <si>
+    <t>10, 20</t>
+  </si>
+  <si>
+    <t>Costl_Arsol_max</t>
+  </si>
+  <si>
+    <t>Costl_Arsol_min</t>
+  </si>
+  <si>
+    <t>Yellow_min</t>
+  </si>
+  <si>
+    <t>Yellow_max</t>
+  </si>
+  <si>
+    <t>VRE1_min</t>
+  </si>
+  <si>
+    <t>VRE1_max</t>
+  </si>
+  <si>
+    <t>VRE2_min</t>
+  </si>
+  <si>
+    <t>VRE2_max</t>
+  </si>
+  <si>
+    <t>VRE3_min</t>
+  </si>
+  <si>
+    <t>VRE3_max</t>
+  </si>
+  <si>
+    <t>NIR1_min</t>
+  </si>
+  <si>
+    <t>NIR1_max</t>
+  </si>
+  <si>
+    <t>NIR2_min</t>
+  </si>
+  <si>
+    <t>NIR2_max</t>
+  </si>
+  <si>
+    <t>WV_min</t>
+  </si>
+  <si>
+    <t>WV_max</t>
+  </si>
+  <si>
+    <t>Cirrus_min</t>
+  </si>
+  <si>
+    <t>Cirrus_max</t>
+  </si>
+  <si>
+    <t>SWIR1_min</t>
+  </si>
+  <si>
+    <t>SWIR1_max</t>
+  </si>
+  <si>
+    <t>SWIR2_min</t>
+  </si>
+  <si>
+    <t>SWIR2_max</t>
+  </si>
+  <si>
+    <t>TIRS1_min</t>
+  </si>
+  <si>
+    <t>TIRS2_min</t>
+  </si>
+  <si>
+    <t>TIRS1_max</t>
+  </si>
+  <si>
+    <t>TIRS2_max</t>
+  </si>
+  <si>
+    <t>Landsat-8</t>
+  </si>
+  <si>
+    <t>30, 15, 100</t>
   </si>
 </sst>
 </file>
@@ -454,25 +590,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0E4EDE-279B-4DA9-9E29-386E11C078C0}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -524,8 +658,11 @@
       <c r="Q1">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -539,10 +676,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -551,34 +688,37 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>
       </c>
       <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
         <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -591,38 +731,38 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>11</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -635,38 +775,38 @@
       <c r="D4">
         <v>0.53700000000000003</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.64600000000000002</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.69399999999999995</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.76700000000000002</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.84799999999999998</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.93100000000000005</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.3380000000000001</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.5389999999999999</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2.0720000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -679,38 +819,38 @@
       <c r="D5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.66500000000000004</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.70399999999999996</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.74</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.78100000000000003</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.83399999999999996</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.86399999999999999</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.94399999999999995</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1.375</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.6120000000000001</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2.194</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -723,38 +863,38 @@
       <c r="D6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.68500000000000005</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.71399999999999997</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.749</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.90800000000000003</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.88100000000000001</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.95799999999999996</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1.4139999999999999</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1.681</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.3119999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -767,38 +907,38 @@
       <c r="D7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3.9E-2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.02</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.14099999999999999</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>2.7E-2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0.14199999999999999</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -811,11 +951,8 @@
       <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>10</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -824,25 +961,28 @@
         <v>20</v>
       </c>
       <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
         <v>10</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>20</v>
-      </c>
-      <c r="K8">
-        <v>60</v>
       </c>
       <c r="L8">
         <v>60</v>
       </c>
       <c r="M8">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -855,32 +995,32 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>6</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>7</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>8</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>10</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -893,32 +1033,32 @@
       <c r="D10">
         <v>0.53300000000000003</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.63600000000000001</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.85099999999999998</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1.363</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1.5669999999999999</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>2.1070000000000002</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.503</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>10.6</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>11.5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -931,32 +1071,32 @@
       <c r="D11">
         <v>0.56100000000000005</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.65500000000000003</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.86499999999999999</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1.373</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1.609</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>2.2010000000000001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.59</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>10.895</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>12.005000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -969,32 +1109,32 @@
       <c r="D12">
         <v>0.59</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.67300000000000004</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.879</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1.3839999999999999</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1.651</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>2.294</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.67600000000000005</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>11.19</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>12.51</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1007,32 +1147,32 @@
       <c r="D13">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.02</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.187</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.17199999999999999</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>0.59</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>1.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1045,13 +1185,10 @@
       <c r="D14">
         <v>30</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>30</v>
       </c>
-      <c r="J14">
-        <v>30</v>
-      </c>
-      <c r="L14">
+      <c r="K14">
         <v>30</v>
       </c>
       <c r="M14">
@@ -1061,16 +1198,19 @@
         <v>30</v>
       </c>
       <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14">
         <v>15</v>
-      </c>
-      <c r="P14">
-        <v>100</v>
       </c>
       <c r="Q14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1080,17 +1220,17 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>4</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1100,17 +1240,17 @@
       <c r="D16">
         <v>0.46</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>0.61799999999999999</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.66700000000000004</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.64</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1120,17 +1260,17 @@
       <c r="D17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.66800000000000004</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.84</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1140,17 +1280,17 @@
       <c r="D18">
         <v>0.66</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>0.71799999999999997</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.76700000000000002</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.04</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1160,109 +1300,1581 @@
       <c r="D19">
         <v>0.2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>0.1</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0.1</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>3</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="D22">
         <v>0.53</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.64</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>0.73</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.77</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="D23">
         <v>0.73</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>0.66</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="D24">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>0.68</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.74</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.81</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="D25">
         <v>0.4</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>0.4</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>0.01</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>0.44</v>
+      </c>
+      <c r="D28">
+        <v>0.52</v>
+      </c>
+      <c r="F28">
+        <v>0.63</v>
+      </c>
+      <c r="G28">
+        <v>0.69</v>
+      </c>
+      <c r="J28">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <f>((C31/2)+C28)</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D29">
+        <f>((D31/2)+D28)</f>
+        <v>0.55499999999999994</v>
+      </c>
+      <c r="F29">
+        <f>((F31/2)+F28)</f>
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="G29">
+        <f>((G31/2)+G28)</f>
+        <v>0.71</v>
+      </c>
+      <c r="J29">
+        <f>((J31/2)+J28)</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>0.51</v>
+      </c>
+      <c r="D30">
+        <v>0.59</v>
+      </c>
+      <c r="F30">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="G30">
+        <v>0.73</v>
+      </c>
+      <c r="J30">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <f>(C30-C28)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D31">
+        <f>(D30-D28)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="F31">
+        <f>(F30-F28)</f>
+        <v>5.5000000000000049E-2</v>
+      </c>
+      <c r="G31">
+        <f>(G30-G28)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J31">
+        <f>(J30-J28)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>0.45</v>
+      </c>
+      <c r="D34">
+        <v>0.52</v>
+      </c>
+      <c r="F34">
+        <v>0.63</v>
+      </c>
+      <c r="J34">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <f>((C37/2)+C34)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D35">
+        <f>((D37/2)+D34)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F35">
+        <f>((F37/2)+F34)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J35">
+        <f>((J37/2)+J34)</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>0.52</v>
+      </c>
+      <c r="D36">
+        <v>0.6</v>
+      </c>
+      <c r="F36">
+        <v>0.69</v>
+      </c>
+      <c r="J36">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <f>(C36-C34)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D37">
+        <f>(D36-D34)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="F37">
+        <f>(F36-F34)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="J37">
+        <f>(J36-J34)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>0.45</v>
+      </c>
+      <c r="D40">
+        <v>0.51</v>
+      </c>
+      <c r="F40">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="J40">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <f>((C43/2)+C40)</f>
+        <v>0.48</v>
+      </c>
+      <c r="D41">
+        <f>((D43/2)+D40)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="F41">
+        <f>((F43/2)+F40)</f>
+        <v>0.67249999999999999</v>
+      </c>
+      <c r="J41">
+        <f>((J43/2)+J40)</f>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <v>0.51</v>
+      </c>
+      <c r="D42">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F42">
+        <v>0.69</v>
+      </c>
+      <c r="J42">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <f>(C42-C40)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D43">
+        <f>(D42-D40)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="F43">
+        <f>(F42-F40)</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="J43">
+        <f>(J42-J40)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>1.65</v>
+      </c>
+      <c r="D44">
+        <v>1.65</v>
+      </c>
+      <c r="F44">
+        <v>1.65</v>
+      </c>
+      <c r="J44">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D46">
+        <v>0.5</v>
+      </c>
+      <c r="F46">
+        <v>0.59</v>
+      </c>
+      <c r="J46">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <f>((C49/2)+C46)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D47">
+        <f>((D49/2)+D46)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="F47">
+        <f>((F49/2)+F46)</f>
+        <v>0.63</v>
+      </c>
+      <c r="J47">
+        <f>((J49/2)+J46)</f>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D48">
+        <v>0.59</v>
+      </c>
+      <c r="F48">
+        <v>0.67</v>
+      </c>
+      <c r="J48">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <f>(C48-C46)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D49">
+        <f>(D48-D46)</f>
+        <v>8.9999999999999969E-2</v>
+      </c>
+      <c r="F49">
+        <f>(F48-F46)</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="J49">
+        <f>(J48-J46)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>0.45</v>
+      </c>
+      <c r="D52">
+        <v>0.53</v>
+      </c>
+      <c r="F52">
+        <v>0.625</v>
+      </c>
+      <c r="J52">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <f>((C55/2)+C52)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D53">
+        <f>((D55/2)+D52)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F53">
+        <f>((F55/2)+F52)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J53">
+        <f>((J55/2)+J52)</f>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>0.52</v>
+      </c>
+      <c r="D54">
+        <v>0.59</v>
+      </c>
+      <c r="F54">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="J54">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <f>(C54-C52)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D55">
+        <f>(D54-D52)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="F55">
+        <f>(F54-F52)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="J55">
+        <f>(J54-J52)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>0.45</v>
+      </c>
+      <c r="D58">
+        <v>0.52</v>
+      </c>
+      <c r="F58">
+        <v>0.63</v>
+      </c>
+      <c r="J58">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <f>((C61/2)+C58)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D59">
+        <f>((D61/2)+D58)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F59">
+        <f>((F61/2)+F58)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J59">
+        <f>((J61/2)+J58)</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <v>0.52</v>
+      </c>
+      <c r="D60">
+        <v>0.6</v>
+      </c>
+      <c r="F60">
+        <v>0.69</v>
+      </c>
+      <c r="J60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61">
+        <f>(C60-C58)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D61">
+        <f>(D60-D58)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="F61">
+        <f>(F60-F58)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="J61">
+        <f>(J60-J58)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>6</v>
+      </c>
+      <c r="K63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
+        <v>0.4</v>
+      </c>
+      <c r="C64">
+        <v>0.45</v>
+      </c>
+      <c r="D64">
+        <v>0.51</v>
+      </c>
+      <c r="E64">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F64">
+        <v>0.63</v>
+      </c>
+      <c r="H64">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="K64">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65">
+        <f>((B67/2)+B64)</f>
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="C65">
+        <f>((C67/2)+C64)</f>
+        <v>0.48</v>
+      </c>
+      <c r="D65">
+        <f>((D67/2)+D64)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="E65">
+        <f>((E67/2)+E64)</f>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F65">
+        <f>((F67/2)+F64)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="H65">
+        <f>((H67/2)+H64)</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K65">
+        <f>((K67/2)+K64)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66">
+        <v>0.45</v>
+      </c>
+      <c r="C66">
+        <v>0.51</v>
+      </c>
+      <c r="D66">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E66">
+        <v>0.625</v>
+      </c>
+      <c r="F66">
+        <v>0.69</v>
+      </c>
+      <c r="H66">
+        <v>0.745</v>
+      </c>
+      <c r="K66">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67">
+        <f>(B66-B64)</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="C67">
+        <f>(C66-C64)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D67">
+        <f>(D66-D64)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="E67">
+        <f>(E66-E64)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F67">
+        <f>(F66-F64)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="H67">
+        <f>(H66-H64)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="K67">
+        <f>(K66-K64)</f>
+        <v>0.18000000000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68">
+        <v>1.84</v>
+      </c>
+      <c r="C68">
+        <v>1.84</v>
+      </c>
+      <c r="D68">
+        <v>1.84</v>
+      </c>
+      <c r="E68">
+        <v>1.84</v>
+      </c>
+      <c r="F68">
+        <v>1.84</v>
+      </c>
+      <c r="H68">
+        <v>1.84</v>
+      </c>
+      <c r="K68">
+        <v>1.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA4A52-2D86-4CA5-B69D-2CE7880AF49C}">
+  <dimension ref="A1:AH12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N34" sqref="L34:N46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5703125" customWidth="1"/>
+    <col min="30" max="30" width="12" customWidth="1"/>
+    <col min="31" max="31" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E2">
+        <v>0.439</v>
+      </c>
+      <c r="F2">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="G2">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H2">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="K2">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="L2">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="M2">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="N2">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="O2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="P2">
+        <v>0.749</v>
+      </c>
+      <c r="Q2">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="R2">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="S2">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="T2">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="U2">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="V2">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="W2">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="X2">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="Y2">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="Z2">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AA2">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="AB2">
+        <v>1.681</v>
+      </c>
+      <c r="AC2">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="AD2">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="AE2">
+        <v>10.6</v>
+      </c>
+      <c r="AF2">
+        <v>11.19</v>
+      </c>
+      <c r="AG2">
+        <v>11.5</v>
+      </c>
+      <c r="AH2">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <v>0.435</v>
+      </c>
+      <c r="D3">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.59</v>
+      </c>
+      <c r="K3">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="L3">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="U3">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="V3">
+        <v>0.879</v>
+      </c>
+      <c r="Y3">
+        <v>1.363</v>
+      </c>
+      <c r="Z3">
+        <v>1.3839999999999999</v>
+      </c>
+      <c r="AA3">
+        <v>1.5669999999999999</v>
+      </c>
+      <c r="AB3">
+        <v>1.651</v>
+      </c>
+      <c r="AC3">
+        <v>2.1070000000000002</v>
+      </c>
+      <c r="AD3">
+        <v>2.294</v>
+      </c>
+      <c r="AE3">
+        <v>10.6</v>
+      </c>
+      <c r="AF3">
+        <v>11.19</v>
+      </c>
+      <c r="AG3">
+        <v>11</v>
+      </c>
+      <c r="AH3">
+        <v>12.005000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0.375</v>
+      </c>
+      <c r="F4">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G4">
+        <v>0.46</v>
+      </c>
+      <c r="H4">
+        <v>0.66</v>
+      </c>
+      <c r="K4">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="L4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="O4">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="P4">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="S4">
+        <v>0.64</v>
+      </c>
+      <c r="T4">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
+      </c>
+      <c r="G5">
+        <v>0.53</v>
+      </c>
+      <c r="H5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.64</v>
+      </c>
+      <c r="L5">
+        <v>0.68</v>
+      </c>
+      <c r="O5">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.74</v>
+      </c>
+      <c r="S5">
+        <v>0.77</v>
+      </c>
+      <c r="T5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0.44</v>
+      </c>
+      <c r="F6">
+        <v>0.51</v>
+      </c>
+      <c r="G6">
+        <v>0.52</v>
+      </c>
+      <c r="H6">
+        <v>0.59</v>
+      </c>
+      <c r="K6">
+        <v>0.63</v>
+      </c>
+      <c r="L6">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="M6">
+        <v>0.71</v>
+      </c>
+      <c r="N6">
+        <v>0.73</v>
+      </c>
+      <c r="S6">
+        <v>0.76</v>
+      </c>
+      <c r="T6">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0.45</v>
+      </c>
+      <c r="F7">
+        <v>0.52</v>
+      </c>
+      <c r="G7">
+        <v>0.52</v>
+      </c>
+      <c r="H7">
+        <v>0.6</v>
+      </c>
+      <c r="K7">
+        <v>0.66</v>
+      </c>
+      <c r="L7">
+        <v>0.69</v>
+      </c>
+      <c r="S7">
+        <v>0.76</v>
+      </c>
+      <c r="T7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>1.65</v>
+      </c>
+      <c r="E8">
+        <v>0.45</v>
+      </c>
+      <c r="F8">
+        <v>0.51</v>
+      </c>
+      <c r="G8">
+        <v>0.51</v>
+      </c>
+      <c r="H8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K8">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="L8">
+        <v>0.69</v>
+      </c>
+      <c r="S8">
+        <v>0.78</v>
+      </c>
+      <c r="T8">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>0.59</v>
+      </c>
+      <c r="K9">
+        <v>0.59</v>
+      </c>
+      <c r="L9">
+        <v>0.67</v>
+      </c>
+      <c r="S9">
+        <v>0.78</v>
+      </c>
+      <c r="T9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0.45</v>
+      </c>
+      <c r="F10">
+        <v>0.52</v>
+      </c>
+      <c r="G10">
+        <v>0.53</v>
+      </c>
+      <c r="H10">
+        <v>0.59</v>
+      </c>
+      <c r="K10">
+        <v>0.625</v>
+      </c>
+      <c r="L10">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="S10">
+        <v>0.76</v>
+      </c>
+      <c r="T10">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.45</v>
+      </c>
+      <c r="F11">
+        <v>0.52</v>
+      </c>
+      <c r="G11">
+        <v>0.52</v>
+      </c>
+      <c r="H11">
+        <v>0.6</v>
+      </c>
+      <c r="K11">
+        <v>0.63</v>
+      </c>
+      <c r="L11">
+        <v>0.69</v>
+      </c>
+      <c r="S11">
+        <v>0.76</v>
+      </c>
+      <c r="T11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>1.84</v>
+      </c>
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12">
+        <v>0.45</v>
+      </c>
+      <c r="E12">
+        <v>0.45</v>
+      </c>
+      <c r="F12">
+        <v>0.51</v>
+      </c>
+      <c r="G12">
+        <v>0.51</v>
+      </c>
+      <c r="H12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J12">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.63</v>
+      </c>
+      <c r="L12">
+        <v>0.69</v>
+      </c>
+      <c r="O12">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="P12">
+        <v>0.745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table - Bands Sensors Fixed
New version of bands sensor
</commit_message>
<xml_diff>
--- a/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
+++ b/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Repos\StopCortaderiaLife\DATA\TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C51FF72F-6D3C-477A-8FE7-AD1CF5299D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0DEBCF-E2A4-488E-9355-BB51FC3FB4C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
   <si>
     <t>Blue</t>
   </si>
@@ -99,10 +100,145 @@
     <t>RedEdgeMx</t>
   </si>
   <si>
-    <t>Res (m)(a 120m)</t>
-  </si>
-  <si>
     <t>Parrot Sequoia</t>
+  </si>
+  <si>
+    <t>RapidEye</t>
+  </si>
+  <si>
+    <t>Ikonos</t>
+  </si>
+  <si>
+    <t>Geoeye 1</t>
+  </si>
+  <si>
+    <t>Planet - Dove 1 to 4</t>
+  </si>
+  <si>
+    <t>SPOT 6 and 7</t>
+  </si>
+  <si>
+    <t>Kompsat 2, 3 and 3A</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Worldview-2 and 3</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Spatial_res</t>
+  </si>
+  <si>
+    <t>Blue_min</t>
+  </si>
+  <si>
+    <t>Blue_max</t>
+  </si>
+  <si>
+    <t>Green_min</t>
+  </si>
+  <si>
+    <t>Green_max</t>
+  </si>
+  <si>
+    <t>Red_min</t>
+  </si>
+  <si>
+    <t>Red_max</t>
+  </si>
+  <si>
+    <t>Sentinel-2</t>
+  </si>
+  <si>
+    <t>10, 20</t>
+  </si>
+  <si>
+    <t>Costl_Arsol_max</t>
+  </si>
+  <si>
+    <t>Costl_Arsol_min</t>
+  </si>
+  <si>
+    <t>Yellow_min</t>
+  </si>
+  <si>
+    <t>Yellow_max</t>
+  </si>
+  <si>
+    <t>VRE1_min</t>
+  </si>
+  <si>
+    <t>VRE1_max</t>
+  </si>
+  <si>
+    <t>VRE2_min</t>
+  </si>
+  <si>
+    <t>VRE2_max</t>
+  </si>
+  <si>
+    <t>VRE3_min</t>
+  </si>
+  <si>
+    <t>VRE3_max</t>
+  </si>
+  <si>
+    <t>NIR1_min</t>
+  </si>
+  <si>
+    <t>NIR1_max</t>
+  </si>
+  <si>
+    <t>NIR2_min</t>
+  </si>
+  <si>
+    <t>NIR2_max</t>
+  </si>
+  <si>
+    <t>WV_min</t>
+  </si>
+  <si>
+    <t>WV_max</t>
+  </si>
+  <si>
+    <t>Cirrus_min</t>
+  </si>
+  <si>
+    <t>Cirrus_max</t>
+  </si>
+  <si>
+    <t>SWIR1_min</t>
+  </si>
+  <si>
+    <t>SWIR1_max</t>
+  </si>
+  <si>
+    <t>SWIR2_min</t>
+  </si>
+  <si>
+    <t>SWIR2_max</t>
+  </si>
+  <si>
+    <t>TIRS1_min</t>
+  </si>
+  <si>
+    <t>TIRS2_min</t>
+  </si>
+  <si>
+    <t>TIRS1_max</t>
+  </si>
+  <si>
+    <t>TIRS2_max</t>
+  </si>
+  <si>
+    <t>Landsat-8</t>
+  </si>
+  <si>
+    <t>30, 15, 100</t>
   </si>
 </sst>
 </file>
@@ -454,25 +590,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0E4EDE-279B-4DA9-9E29-386E11C078C0}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -524,8 +658,11 @@
       <c r="Q1">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -539,10 +676,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -551,34 +688,37 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>
       </c>
       <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
         <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -591,38 +731,38 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>11</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -635,38 +775,38 @@
       <c r="D4">
         <v>0.53700000000000003</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.64600000000000002</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.69399999999999995</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.76700000000000002</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.84799999999999998</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.93100000000000005</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.3380000000000001</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.5389999999999999</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2.0720000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -679,38 +819,38 @@
       <c r="D5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.66500000000000004</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.70399999999999996</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.74</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.78100000000000003</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.83399999999999996</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.86399999999999999</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.94399999999999995</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1.375</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.6120000000000001</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2.194</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -723,38 +863,38 @@
       <c r="D6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.68500000000000005</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.71399999999999997</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.749</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.79600000000000004</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.90800000000000003</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.88100000000000001</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.95799999999999996</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1.4139999999999999</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1.681</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2.3119999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -767,38 +907,38 @@
       <c r="D7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3.9E-2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.02</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.14099999999999999</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>2.7E-2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0.14199999999999999</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -811,11 +951,8 @@
       <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>10</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -824,25 +961,28 @@
         <v>20</v>
       </c>
       <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
         <v>10</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>20</v>
-      </c>
-      <c r="K8">
-        <v>60</v>
       </c>
       <c r="L8">
         <v>60</v>
       </c>
       <c r="M8">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -855,32 +995,32 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>6</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>7</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>8</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>10</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -893,32 +1033,32 @@
       <c r="D10">
         <v>0.53300000000000003</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.63600000000000001</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.85099999999999998</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1.363</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1.5669999999999999</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>2.1070000000000002</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.503</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>10.6</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>11.5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -931,32 +1071,32 @@
       <c r="D11">
         <v>0.56100000000000005</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.65500000000000003</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.86499999999999999</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1.373</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1.609</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>2.2010000000000001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.59</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>10.895</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>12.005000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -969,32 +1109,32 @@
       <c r="D12">
         <v>0.59</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.67300000000000004</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.879</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1.3839999999999999</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1.651</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>2.294</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.67600000000000005</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>11.19</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>12.51</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1007,32 +1147,32 @@
       <c r="D13">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.02</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.187</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.17199999999999999</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>0.59</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>1.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1045,13 +1185,10 @@
       <c r="D14">
         <v>30</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>30</v>
       </c>
-      <c r="J14">
-        <v>30</v>
-      </c>
-      <c r="L14">
+      <c r="K14">
         <v>30</v>
       </c>
       <c r="M14">
@@ -1061,16 +1198,19 @@
         <v>30</v>
       </c>
       <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14">
         <v>15</v>
-      </c>
-      <c r="P14">
-        <v>100</v>
       </c>
       <c r="Q14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1080,17 +1220,17 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>4</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1100,17 +1240,17 @@
       <c r="D16">
         <v>0.46</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>0.61799999999999999</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.66700000000000004</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.64</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1120,17 +1260,17 @@
       <c r="D17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.66800000000000004</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.84</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1140,17 +1280,17 @@
       <c r="D18">
         <v>0.66</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>0.71799999999999997</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.76700000000000002</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.04</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1160,109 +1300,1581 @@
       <c r="D19">
         <v>0.2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>0.1</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0.1</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>3</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="D22">
         <v>0.53</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.64</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>0.73</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.77</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="D23">
         <v>0.73</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>0.66</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="D24">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>0.68</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.74</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.81</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="D25">
         <v>0.4</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>0.4</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>0.01</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>0.44</v>
+      </c>
+      <c r="D28">
+        <v>0.52</v>
+      </c>
+      <c r="F28">
+        <v>0.63</v>
+      </c>
+      <c r="G28">
+        <v>0.69</v>
+      </c>
+      <c r="J28">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <f>((C31/2)+C28)</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D29">
+        <f>((D31/2)+D28)</f>
+        <v>0.55499999999999994</v>
+      </c>
+      <c r="F29">
+        <f>((F31/2)+F28)</f>
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="G29">
+        <f>((G31/2)+G28)</f>
+        <v>0.71</v>
+      </c>
+      <c r="J29">
+        <f>((J31/2)+J28)</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>0.51</v>
+      </c>
+      <c r="D30">
+        <v>0.59</v>
+      </c>
+      <c r="F30">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="G30">
+        <v>0.73</v>
+      </c>
+      <c r="J30">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <f>(C30-C28)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D31">
+        <f>(D30-D28)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="F31">
+        <f>(F30-F28)</f>
+        <v>5.5000000000000049E-2</v>
+      </c>
+      <c r="G31">
+        <f>(G30-G28)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J31">
+        <f>(J30-J28)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>0.45</v>
+      </c>
+      <c r="D34">
+        <v>0.52</v>
+      </c>
+      <c r="F34">
+        <v>0.63</v>
+      </c>
+      <c r="J34">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <f>((C37/2)+C34)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D35">
+        <f>((D37/2)+D34)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F35">
+        <f>((F37/2)+F34)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J35">
+        <f>((J37/2)+J34)</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>0.52</v>
+      </c>
+      <c r="D36">
+        <v>0.6</v>
+      </c>
+      <c r="F36">
+        <v>0.69</v>
+      </c>
+      <c r="J36">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <f>(C36-C34)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D37">
+        <f>(D36-D34)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="F37">
+        <f>(F36-F34)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="J37">
+        <f>(J36-J34)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>0.45</v>
+      </c>
+      <c r="D40">
+        <v>0.51</v>
+      </c>
+      <c r="F40">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="J40">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <f>((C43/2)+C40)</f>
+        <v>0.48</v>
+      </c>
+      <c r="D41">
+        <f>((D43/2)+D40)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="F41">
+        <f>((F43/2)+F40)</f>
+        <v>0.67249999999999999</v>
+      </c>
+      <c r="J41">
+        <f>((J43/2)+J40)</f>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <v>0.51</v>
+      </c>
+      <c r="D42">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F42">
+        <v>0.69</v>
+      </c>
+      <c r="J42">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <f>(C42-C40)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D43">
+        <f>(D42-D40)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="F43">
+        <f>(F42-F40)</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="J43">
+        <f>(J42-J40)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>1.65</v>
+      </c>
+      <c r="D44">
+        <v>1.65</v>
+      </c>
+      <c r="F44">
+        <v>1.65</v>
+      </c>
+      <c r="J44">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D46">
+        <v>0.5</v>
+      </c>
+      <c r="F46">
+        <v>0.59</v>
+      </c>
+      <c r="J46">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <f>((C49/2)+C46)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D47">
+        <f>((D49/2)+D46)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="F47">
+        <f>((F49/2)+F46)</f>
+        <v>0.63</v>
+      </c>
+      <c r="J47">
+        <f>((J49/2)+J46)</f>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D48">
+        <v>0.59</v>
+      </c>
+      <c r="F48">
+        <v>0.67</v>
+      </c>
+      <c r="J48">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <f>(C48-C46)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D49">
+        <f>(D48-D46)</f>
+        <v>8.9999999999999969E-2</v>
+      </c>
+      <c r="F49">
+        <f>(F48-F46)</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="J49">
+        <f>(J48-J46)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>0.45</v>
+      </c>
+      <c r="D52">
+        <v>0.53</v>
+      </c>
+      <c r="F52">
+        <v>0.625</v>
+      </c>
+      <c r="J52">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <f>((C55/2)+C52)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D53">
+        <f>((D55/2)+D52)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F53">
+        <f>((F55/2)+F52)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J53">
+        <f>((J55/2)+J52)</f>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>0.52</v>
+      </c>
+      <c r="D54">
+        <v>0.59</v>
+      </c>
+      <c r="F54">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="J54">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <f>(C54-C52)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D55">
+        <f>(D54-D52)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="F55">
+        <f>(F54-F52)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="J55">
+        <f>(J54-J52)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>0.45</v>
+      </c>
+      <c r="D58">
+        <v>0.52</v>
+      </c>
+      <c r="F58">
+        <v>0.63</v>
+      </c>
+      <c r="J58">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <f>((C61/2)+C58)</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D59">
+        <f>((D61/2)+D58)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F59">
+        <f>((F61/2)+F58)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J59">
+        <f>((J61/2)+J58)</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <v>0.52</v>
+      </c>
+      <c r="D60">
+        <v>0.6</v>
+      </c>
+      <c r="F60">
+        <v>0.69</v>
+      </c>
+      <c r="J60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61">
+        <f>(C60-C58)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D61">
+        <f>(D60-D58)</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+      <c r="F61">
+        <f>(F60-F58)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="J61">
+        <f>(J60-J58)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>6</v>
+      </c>
+      <c r="K63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
+        <v>0.4</v>
+      </c>
+      <c r="C64">
+        <v>0.45</v>
+      </c>
+      <c r="D64">
+        <v>0.51</v>
+      </c>
+      <c r="E64">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F64">
+        <v>0.63</v>
+      </c>
+      <c r="H64">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="K64">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65">
+        <f>((B67/2)+B64)</f>
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="C65">
+        <f>((C67/2)+C64)</f>
+        <v>0.48</v>
+      </c>
+      <c r="D65">
+        <f>((D67/2)+D64)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="E65">
+        <f>((E67/2)+E64)</f>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F65">
+        <f>((F67/2)+F64)</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="H65">
+        <f>((H67/2)+H64)</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K65">
+        <f>((K67/2)+K64)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66">
+        <v>0.45</v>
+      </c>
+      <c r="C66">
+        <v>0.51</v>
+      </c>
+      <c r="D66">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E66">
+        <v>0.625</v>
+      </c>
+      <c r="F66">
+        <v>0.69</v>
+      </c>
+      <c r="H66">
+        <v>0.745</v>
+      </c>
+      <c r="K66">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67">
+        <f>(B66-B64)</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="C67">
+        <f>(C66-C64)</f>
+        <v>0.06</v>
+      </c>
+      <c r="D67">
+        <f>(D66-D64)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="E67">
+        <f>(E66-E64)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F67">
+        <f>(F66-F64)</f>
+        <v>5.9999999999999942E-2</v>
+      </c>
+      <c r="H67">
+        <f>(H66-H64)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="K67">
+        <f>(K66-K64)</f>
+        <v>0.18000000000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68">
+        <v>1.84</v>
+      </c>
+      <c r="C68">
+        <v>1.84</v>
+      </c>
+      <c r="D68">
+        <v>1.84</v>
+      </c>
+      <c r="E68">
+        <v>1.84</v>
+      </c>
+      <c r="F68">
+        <v>1.84</v>
+      </c>
+      <c r="H68">
+        <v>1.84</v>
+      </c>
+      <c r="K68">
+        <v>1.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA4A52-2D86-4CA5-B69D-2CE7880AF49C}">
+  <dimension ref="A1:AH12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N34" sqref="L34:N46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5703125" customWidth="1"/>
+    <col min="30" max="30" width="12" customWidth="1"/>
+    <col min="31" max="31" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E2">
+        <v>0.439</v>
+      </c>
+      <c r="F2">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="G2">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H2">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="K2">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="L2">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="M2">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="N2">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="O2">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="P2">
+        <v>0.749</v>
+      </c>
+      <c r="Q2">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="R2">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="S2">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="T2">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="U2">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="V2">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="W2">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="X2">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="Y2">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="Z2">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="AA2">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="AB2">
+        <v>1.681</v>
+      </c>
+      <c r="AC2">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="AD2">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="AE2">
+        <v>10.6</v>
+      </c>
+      <c r="AF2">
+        <v>11.19</v>
+      </c>
+      <c r="AG2">
+        <v>11.5</v>
+      </c>
+      <c r="AH2">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <v>0.435</v>
+      </c>
+      <c r="D3">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.59</v>
+      </c>
+      <c r="K3">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="L3">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="U3">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="V3">
+        <v>0.879</v>
+      </c>
+      <c r="Y3">
+        <v>1.363</v>
+      </c>
+      <c r="Z3">
+        <v>1.3839999999999999</v>
+      </c>
+      <c r="AA3">
+        <v>1.5669999999999999</v>
+      </c>
+      <c r="AB3">
+        <v>1.651</v>
+      </c>
+      <c r="AC3">
+        <v>2.1070000000000002</v>
+      </c>
+      <c r="AD3">
+        <v>2.294</v>
+      </c>
+      <c r="AE3">
+        <v>10.6</v>
+      </c>
+      <c r="AF3">
+        <v>11.19</v>
+      </c>
+      <c r="AG3">
+        <v>11</v>
+      </c>
+      <c r="AH3">
+        <v>12.005000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0.375</v>
+      </c>
+      <c r="F4">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G4">
+        <v>0.46</v>
+      </c>
+      <c r="H4">
+        <v>0.66</v>
+      </c>
+      <c r="K4">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="L4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="O4">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="P4">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="S4">
+        <v>0.64</v>
+      </c>
+      <c r="T4">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
+      </c>
+      <c r="G5">
+        <v>0.53</v>
+      </c>
+      <c r="H5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.64</v>
+      </c>
+      <c r="L5">
+        <v>0.68</v>
+      </c>
+      <c r="O5">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.74</v>
+      </c>
+      <c r="S5">
+        <v>0.77</v>
+      </c>
+      <c r="T5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0.44</v>
+      </c>
+      <c r="F6">
+        <v>0.51</v>
+      </c>
+      <c r="G6">
+        <v>0.52</v>
+      </c>
+      <c r="H6">
+        <v>0.59</v>
+      </c>
+      <c r="K6">
+        <v>0.63</v>
+      </c>
+      <c r="L6">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="M6">
+        <v>0.71</v>
+      </c>
+      <c r="N6">
+        <v>0.73</v>
+      </c>
+      <c r="S6">
+        <v>0.76</v>
+      </c>
+      <c r="T6">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0.45</v>
+      </c>
+      <c r="F7">
+        <v>0.52</v>
+      </c>
+      <c r="G7">
+        <v>0.52</v>
+      </c>
+      <c r="H7">
+        <v>0.6</v>
+      </c>
+      <c r="K7">
+        <v>0.66</v>
+      </c>
+      <c r="L7">
+        <v>0.69</v>
+      </c>
+      <c r="S7">
+        <v>0.76</v>
+      </c>
+      <c r="T7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>1.65</v>
+      </c>
+      <c r="E8">
+        <v>0.45</v>
+      </c>
+      <c r="F8">
+        <v>0.51</v>
+      </c>
+      <c r="G8">
+        <v>0.51</v>
+      </c>
+      <c r="H8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K8">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="L8">
+        <v>0.69</v>
+      </c>
+      <c r="S8">
+        <v>0.78</v>
+      </c>
+      <c r="T8">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>0.59</v>
+      </c>
+      <c r="K9">
+        <v>0.59</v>
+      </c>
+      <c r="L9">
+        <v>0.67</v>
+      </c>
+      <c r="S9">
+        <v>0.78</v>
+      </c>
+      <c r="T9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0.45</v>
+      </c>
+      <c r="F10">
+        <v>0.52</v>
+      </c>
+      <c r="G10">
+        <v>0.53</v>
+      </c>
+      <c r="H10">
+        <v>0.59</v>
+      </c>
+      <c r="K10">
+        <v>0.625</v>
+      </c>
+      <c r="L10">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="S10">
+        <v>0.76</v>
+      </c>
+      <c r="T10">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.45</v>
+      </c>
+      <c r="F11">
+        <v>0.52</v>
+      </c>
+      <c r="G11">
+        <v>0.52</v>
+      </c>
+      <c r="H11">
+        <v>0.6</v>
+      </c>
+      <c r="K11">
+        <v>0.63</v>
+      </c>
+      <c r="L11">
+        <v>0.69</v>
+      </c>
+      <c r="S11">
+        <v>0.76</v>
+      </c>
+      <c r="T11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>1.84</v>
+      </c>
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12">
+        <v>0.45</v>
+      </c>
+      <c r="E12">
+        <v>0.45</v>
+      </c>
+      <c r="F12">
+        <v>0.51</v>
+      </c>
+      <c r="G12">
+        <v>0.51</v>
+      </c>
+      <c r="H12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J12">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.63</v>
+      </c>
+      <c r="L12">
+        <v>0.69</v>
+      </c>
+      <c r="O12">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="P12">
+        <v>0.745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R Code for Sensor and Master tables
R Code for Sensor and wl with wordlview 3 actualized.
</commit_message>
<xml_diff>
--- a/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
+++ b/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Repos\StopCortaderiaLife\DATA\TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0DEBCF-E2A4-488E-9355-BB51FC3FB4C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138F6C0-839D-42A9-9E07-AC2A3C32EC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>Blue</t>
   </si>
@@ -239,6 +239,45 @@
   </si>
   <si>
     <t>30, 15, 100</t>
+  </si>
+  <si>
+    <t>SWIR3_min</t>
+  </si>
+  <si>
+    <t>SWIR3_max</t>
+  </si>
+  <si>
+    <t>SWIR4_min</t>
+  </si>
+  <si>
+    <t>SWIR4_max</t>
+  </si>
+  <si>
+    <t>SWIR5_min</t>
+  </si>
+  <si>
+    <t>SWIR5_max</t>
+  </si>
+  <si>
+    <t>SWIR6_min</t>
+  </si>
+  <si>
+    <t>SWIR6_max</t>
+  </si>
+  <si>
+    <t>SWIR7_min</t>
+  </si>
+  <si>
+    <t>SWIR7_max</t>
+  </si>
+  <si>
+    <t>Worldview-2</t>
+  </si>
+  <si>
+    <t>Worldview-3</t>
+  </si>
+  <si>
+    <t>1.24,3.7</t>
   </si>
 </sst>
 </file>
@@ -2259,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA4A52-2D86-4CA5-B69D-2CE7880AF49C}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AR13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="L34:N46"/>
+      <selection sqref="A1:AR13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,7 +2340,7 @@
     <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -2393,19 +2432,49 @@
         <v>62</v>
       </c>
       <c r="AE1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO1" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AP1" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AQ1" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AR1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2484,26 +2553,26 @@
       <c r="AB2">
         <v>1.681</v>
       </c>
-      <c r="AC2">
+      <c r="AG2">
         <v>2.0720000000000001</v>
       </c>
-      <c r="AD2">
+      <c r="AH2">
         <v>2.3119999999999998</v>
       </c>
-      <c r="AE2">
+      <c r="AO2">
         <v>10.6</v>
       </c>
-      <c r="AF2">
+      <c r="AP2">
         <v>11.19</v>
       </c>
-      <c r="AG2">
+      <c r="AQ2">
         <v>11.5</v>
       </c>
-      <c r="AH2">
+      <c r="AR2">
         <v>12.51</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2552,26 +2621,26 @@
       <c r="AB3">
         <v>1.651</v>
       </c>
-      <c r="AC3">
+      <c r="AG3">
         <v>2.1070000000000002</v>
       </c>
-      <c r="AD3">
+      <c r="AH3">
         <v>2.294</v>
       </c>
-      <c r="AE3">
+      <c r="AO3">
         <v>10.6</v>
       </c>
-      <c r="AF3">
+      <c r="AP3">
         <v>11.19</v>
       </c>
-      <c r="AG3">
+      <c r="AQ3">
         <v>11</v>
       </c>
-      <c r="AH3">
+      <c r="AR3">
         <v>12.005000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2606,7 +2675,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2635,7 +2704,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2673,7 +2742,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2705,7 +2774,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2737,7 +2806,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2838,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2801,7 +2870,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2826,6 +2895,12 @@
       <c r="L11">
         <v>0.69</v>
       </c>
+      <c r="O11">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="P11">
+        <v>0.745</v>
+      </c>
       <c r="S11">
         <v>0.76</v>
       </c>
@@ -2833,9 +2908,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>1.84</v>
@@ -2859,10 +2934,10 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I12">
-        <v>0.57999999999999996</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="J12">
-        <v>0.60499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="K12">
         <v>0.63</v>
@@ -2875,6 +2950,119 @@
       </c>
       <c r="P12">
         <v>0.745</v>
+      </c>
+      <c r="S12">
+        <v>0.77</v>
+      </c>
+      <c r="T12">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="U12">
+        <v>0.86</v>
+      </c>
+      <c r="V12">
+        <v>1.04</v>
+      </c>
+      <c r="Y12">
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="Z12">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="AA12">
+        <v>1.55</v>
+      </c>
+      <c r="AB12">
+        <v>1.59</v>
+      </c>
+      <c r="AC12">
+        <v>1.64</v>
+      </c>
+      <c r="AD12">
+        <v>1.68</v>
+      </c>
+      <c r="AE12">
+        <v>1.71</v>
+      </c>
+      <c r="AF12">
+        <v>1.75</v>
+      </c>
+      <c r="AG12">
+        <v>2.145</v>
+      </c>
+      <c r="AH12">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="AI12">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="AJ12">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="AK12">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="AL12">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="AM12">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="AN12">
+        <v>2.3650000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13">
+        <v>0.4</v>
+      </c>
+      <c r="D13">
+        <v>0.45</v>
+      </c>
+      <c r="E13">
+        <v>0.45</v>
+      </c>
+      <c r="F13">
+        <v>0.51</v>
+      </c>
+      <c r="G13">
+        <v>0.51</v>
+      </c>
+      <c r="H13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K13">
+        <v>0.63</v>
+      </c>
+      <c r="L13">
+        <v>0.69</v>
+      </c>
+      <c r="O13">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="P13">
+        <v>0.745</v>
+      </c>
+      <c r="S13">
+        <v>0.77</v>
+      </c>
+      <c r="T13">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="U13">
+        <v>0.86</v>
+      </c>
+      <c r="V13">
+        <v>1.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worldview 2 and 3 fixed
The mistake of worldview 2 and 3 was fixed
</commit_message>
<xml_diff>
--- a/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
+++ b/DATA/TABLES/BandsSensors_2019_24_10_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\Repos\StopCortaderiaLife\DATA\TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138F6C0-839D-42A9-9E07-AC2A3C32EC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45A91AE-811D-4A00-9C57-302BDAB666B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2BC0E692-8C36-4AC6-BD6F-56632CABCA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -2301,7 +2301,7 @@
   <dimension ref="A1:AR13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:AR13"/>
+      <selection activeCell="C12" sqref="C12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,10 +2934,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I12">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="J12">
-        <v>0.625</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K12">
         <v>0.63</v>
@@ -2962,54 +2959,6 @@
       </c>
       <c r="V12">
         <v>1.04</v>
-      </c>
-      <c r="Y12">
-        <v>1.1950000000000001</v>
-      </c>
-      <c r="Z12">
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="AA12">
-        <v>1.55</v>
-      </c>
-      <c r="AB12">
-        <v>1.59</v>
-      </c>
-      <c r="AC12">
-        <v>1.64</v>
-      </c>
-      <c r="AD12">
-        <v>1.68</v>
-      </c>
-      <c r="AE12">
-        <v>1.71</v>
-      </c>
-      <c r="AF12">
-        <v>1.75</v>
-      </c>
-      <c r="AG12">
-        <v>2.145</v>
-      </c>
-      <c r="AH12">
-        <v>2.1850000000000001</v>
-      </c>
-      <c r="AI12">
-        <v>2.1850000000000001</v>
-      </c>
-      <c r="AJ12">
-        <v>2.2250000000000001</v>
-      </c>
-      <c r="AK12">
-        <v>2.2349999999999999</v>
-      </c>
-      <c r="AL12">
-        <v>2.2850000000000001</v>
-      </c>
-      <c r="AM12">
-        <v>2.2949999999999999</v>
-      </c>
-      <c r="AN12">
-        <v>2.3650000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -3038,7 +2987,10 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I13">
-        <v>0.57999999999999996</v>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="J13">
+        <v>0.625</v>
       </c>
       <c r="K13">
         <v>0.63</v>
@@ -3063,6 +3015,54 @@
       </c>
       <c r="V13">
         <v>1.04</v>
+      </c>
+      <c r="Y13">
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="Z13">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="AA13">
+        <v>1.55</v>
+      </c>
+      <c r="AB13">
+        <v>1.59</v>
+      </c>
+      <c r="AC13">
+        <v>1.64</v>
+      </c>
+      <c r="AD13">
+        <v>1.68</v>
+      </c>
+      <c r="AE13">
+        <v>1.71</v>
+      </c>
+      <c r="AF13">
+        <v>1.75</v>
+      </c>
+      <c r="AG13">
+        <v>2.145</v>
+      </c>
+      <c r="AH13">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="AI13">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="AJ13">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="AK13">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="AL13">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="AM13">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="AN13">
+        <v>2.3650000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>